<commit_message>
time plan, abstract and presentation is updated and will be checked
</commit_message>
<xml_diff>
--- a/tik/timeplan.xlsx
+++ b/tik/timeplan.xlsx
@@ -55,9 +55,6 @@
     <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve">propose a software based dead time compensation method </t>
-  </si>
-  <si>
     <t>submit the results of the proposed method to a conference (*)</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>submit the results of the proposed method to a journal (**)</t>
   </si>
   <si>
-    <t>analyze &amp; investigate the dead-time effect on the VSIs for various PMSMs</t>
-  </si>
-  <si>
     <t>apply the literature compensation methods by experimentally</t>
   </si>
   <si>
@@ -77,6 +71,12 @@
   </si>
   <si>
     <t>improve the method and verify with both simulation and experimental</t>
+  </si>
+  <si>
+    <t>analyze &amp; investigate the nonlineariy effect on the VSIs for various PMSMs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propose a software based nonlinearity compensation method </t>
   </si>
 </sst>
 </file>
@@ -406,15 +406,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -431,46 +422,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,7 +779,7 @@
   <dimension ref="B1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="A18:B18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,89 +790,89 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="15"/>
-      <c r="C2" s="23">
+      <c r="B2" s="28"/>
+      <c r="C2" s="22">
         <v>2018</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="24"/>
-      <c r="J2" s="29">
+      <c r="J2" s="25">
         <v>2019</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="N3" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="28"/>
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12"/>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
@@ -887,13 +887,13 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -908,13 +908,13 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="7"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
@@ -929,13 +929,13 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="7"/>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -950,13 +950,13 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="7"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -971,13 +971,13 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="13"/>
+      <c r="B10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -992,26 +992,26 @@
         <v>12</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="7"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="N11" s="11" t="s">
+      <c r="B11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>